<commit_message>
a range of changes
</commit_message>
<xml_diff>
--- a/data-raw/crops/perennnial_crop_temp_table_summary_29_52020.xlsx
+++ b/data-raw/crops/perennnial_crop_temp_table_summary_29_52020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/ISIMIPData/data-raw/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFC8E22-9266-2D40-AB00-C94ABAAC47D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CBC46D-B720-9145-B042-2EB84A202831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16860" yWindow="16200" windowWidth="27240" windowHeight="16440" xr2:uid="{01F94FA6-79B0-7043-BE17-73DA59222455}"/>
+    <workbookView xWindow="34900" yWindow="22240" windowWidth="27240" windowHeight="16440" xr2:uid="{01F94FA6-79B0-7043-BE17-73DA59222455}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,24 +95,6 @@
     <t>title</t>
   </si>
   <si>
-    <t xml:space="preserve">Grapes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blueberries </t>
-  </si>
-  <si>
-    <t>Apples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cherries </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Almonds </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walnuts </t>
-  </si>
-  <si>
     <t>Vits vinifera</t>
   </si>
   <si>
@@ -129,13 +111,31 @@
   </si>
   <si>
     <t>Prunus dulcis</t>
+  </si>
+  <si>
+    <t>Blueberry</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Cherry</t>
+  </si>
+  <si>
+    <t>Almond</t>
+  </si>
+  <si>
+    <t>Walnut</t>
+  </si>
+  <si>
+    <t>Grape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -146,14 +146,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,10 +171,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -501,12 +492,12 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -522,49 +513,49 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -573,21 +564,21 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -595,43 +586,43 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>31</v>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>